<commit_message>
added Datasets, NLP and Time series work
</commit_message>
<xml_diff>
--- a/Important Links.xlsx
+++ b/Important Links.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F5BAE3-17A1-486F-BF98-4520C8F40EA4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Description</t>
   </si>
@@ -134,11 +135,17 @@
   <si>
     <t>http://www.cs.ccsu.edu/~markov/ccsu_courses/datamining-3.html</t>
   </si>
+  <si>
+    <t>Git Hub Repositories</t>
+  </si>
+  <si>
+    <t>https://github.com/abhat222/Data-Science--Cheat-Sheet</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -280,7 +287,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -303,6 +310,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -583,11 +591,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B370"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -641,8 +649,12 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="9"/>
-      <c r="B7" s="5"/>
+      <c r="A7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="9"/>
@@ -2098,10 +2110,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B6" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B7" r:id="rId3" xr:uid="{F29E54FA-A42C-4948-AE8B-472D328A8453}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>